<commit_message>
excel intermediate week 1
</commit_message>
<xml_diff>
--- a/Visualization/Excel Specialization/Excel Skills for Business Intermediate I/Week 1/Practice Challenge/W1_PracticeChallenge_Bondi.xlsx
+++ b/Visualization/Excel Specialization/Excel Skills for Business Intermediate I/Week 1/Practice Challenge/W1_PracticeChallenge_Bondi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandeep Tukkunor\Desktop\100 Days Of Code\Visualization\Excel Specialization\Excel Skills for Business Intermediate I\Week 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandeep Tukkunor\Desktop\100 Days Of Code\Visualization\Excel Specialization\Excel Skills for Business Intermediate I\Week 1\Practice Challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F3324A-92F6-470B-BCA8-D9E0E9199DAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38DDA4A-AE4F-4CA7-9D99-24151CC50D4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11508" yWindow="-12" windowWidth="11544" windowHeight="6192" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>

</xml_diff>